<commit_message>
QAQC'd Sept 2025 COMPASS Syn Sulfide Data
</commit_message>
<xml_diff>
--- a/Porewater/Sulfide/Synoptic_CB/2025/September/Raw Data/Aquifer_Sept2025_SampleIDs.xlsx
+++ b/Porewater/Sulfide/Synoptic_CB/2025/September/Raw Data/Aquifer_Sept2025_SampleIDs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Biogeochemistry\COMPASS Synoptics\Samples &amp; Data\Porewater\H2S\2025\2025 September\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sinet-my.sharepoint.com/personal/readz_si_edu1/Documents/synoptic-discrete-data/Porewater/Sulfide/Synoptic_CB/2025/September/Raw Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F63143-AE54-48F8-96B0-E4798DEE5943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{97F63143-AE54-48F8-96B0-E4798DEE5943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A075D24-1FD4-4A27-BE00-1E9A0A50D423}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{569BB281-6F4B-4FE0-B4AB-E6E4C5F2A2BE}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{569BB281-6F4B-4FE0-B4AB-E6E4C5F2A2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,39 +36,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Sample_ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
   <si>
     <t>Number</t>
   </si>
   <si>
-    <t>TEMPEST_AqWell_20250904_1300_B</t>
-  </si>
-  <si>
-    <t>TEMPEST_AqWell_20250904_1225_B</t>
-  </si>
-  <si>
-    <t>TEMPEST_AqWell_20250904_1400_B</t>
-  </si>
-  <si>
-    <t>TEMPEST_AqWell_20250904_1400_A</t>
-  </si>
-  <si>
-    <t>TEMPEST_AqWell_20250904_1225_C</t>
-  </si>
-  <si>
-    <t>TEMPEST_AqWell_20250904_1400_C</t>
-  </si>
-  <si>
-    <t>TEMPEST_AqWell_20250904_1225_A</t>
-  </si>
-  <si>
-    <t>TEMPEST_AqWell_20250904_1300_A</t>
-  </si>
-  <si>
-    <t>TEMPEST_AqWell_20250904_1300_C</t>
+    <t>TEMPEST</t>
+  </si>
+  <si>
+    <t>AqWell</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Replicate</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -446,95 +446,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21F8A0B-D2F5-4152-8917-6F457D69F7FD}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="36.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.1796875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>116</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>20250904</v>
+      </c>
+      <c r="E2">
+        <v>1300</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>117</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>20250904</v>
+      </c>
+      <c r="E3">
+        <v>1225</v>
+      </c>
+      <c r="F3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>118</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>20250904</v>
+      </c>
+      <c r="E4">
+        <v>1400</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>119</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>20250904</v>
+      </c>
+      <c r="E5">
+        <v>1400</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>120</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>20250904</v>
+      </c>
+      <c r="E6">
+        <v>1225</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>121</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>20250904</v>
+      </c>
+      <c r="E7">
+        <v>1400</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>122</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>20250904</v>
+      </c>
+      <c r="E8">
+        <v>1225</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>123</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>20250904</v>
+      </c>
+      <c r="E9">
+        <v>1300</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>124</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>20250904</v>
+      </c>
+      <c r="E10">
+        <v>1300</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>